<commit_message>
Edits to boxplots and statistics for authors
</commit_message>
<xml_diff>
--- a/Code/STATISTICS.xlsx
+++ b/Code/STATISTICS.xlsx
@@ -19,7 +19,7 @@
     <t>type</t>
   </si>
   <si>
-    <t>transport</t>
+    <t>group</t>
   </si>
   <si>
     <t>PC</t>
@@ -40,10 +40,10 @@
     <t>h2</t>
   </si>
   <si>
-    <t>alltextures</t>
-  </si>
-  <si>
-    <t>mechanical</t>
+    <t>All Textures</t>
+  </si>
+  <si>
+    <t>Mechanical</t>
   </si>
   <si>
     <t>Aeolian</t>

</xml_diff>